<commit_message>
Updating with Uma's new changes
</commit_message>
<xml_diff>
--- a/HumongousInsuranceAgentsAddin/HumongousInsuranceAgentsAddin/HumongousInsuranceExcelSpreadsheet.xlsx
+++ b/HumongousInsuranceAgentsAddin/HumongousInsuranceAgentsAddin/HumongousInsuranceExcelSpreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\temp\documents\visual studio 2015\Projects\HumongousInsuranceAgentsAddin\HumongousInsuranceAgentsAddin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TEMP\Documents\Visual Studio 2015\Projects\HumongousInsuranceAgentsAddin\HumongousInsuranceAgentsAddin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Agents" sheetId="2" r:id="rId2"/>
     <sheet name="Applicants" sheetId="3" r:id="rId3"/>
     <sheet name="Policies" sheetId="4" r:id="rId4"/>
+    <sheet name="Prospects" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>Humongous Insurance Agency Center</t>
   </si>
@@ -119,15 +120,6 @@
     <t>Term Life</t>
   </si>
   <si>
-    <t>Medical Exam Required?</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Humongous Insurance Agent Center</t>
   </si>
   <si>
@@ -150,6 +142,33 @@
   </si>
   <si>
     <t>SampleRatefor$10000</t>
+  </si>
+  <si>
+    <t>MedicalExamRequired</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Prospects - Master List</t>
+  </si>
+  <si>
+    <t>ApplicantName</t>
+  </si>
+  <si>
+    <t>PolicyName</t>
+  </si>
+  <si>
+    <t>SampleRate</t>
+  </si>
+  <si>
+    <t>InsuranceAmount</t>
+  </si>
+  <si>
+    <t>ApproxMonthlyPayment</t>
   </si>
 </sst>
 </file>
@@ -278,15 +297,120 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="7" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="11" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
       <fill>
@@ -589,34 +713,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="AgentsTable" displayName="AgentsTable" ref="A5:A13" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="AgentsTable" displayName="AgentsTable" ref="A5:A13" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A5:A13"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="AgentName" dataDxfId="16"/>
+    <tableColumn id="1" name="AgentName" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ApplicantsTable" displayName="ApplicantsTable" ref="A5:C17" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ApplicantsTable" displayName="ApplicantsTable" ref="A5:C17" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="A5:C17"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Applicant" dataDxfId="10"/>
-    <tableColumn id="2" name="Age" dataDxfId="9"/>
-    <tableColumn id="3" name="Gender" dataDxfId="8"/>
+    <tableColumn id="1" name="Applicant" dataDxfId="21"/>
+    <tableColumn id="2" name="Age" dataDxfId="20"/>
+    <tableColumn id="3" name="Gender" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="PoliciesTable" displayName="PoliciesTable" ref="A5:C9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="PoliciesTable" displayName="PoliciesTable" ref="A5:C9" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A5:C9"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Policy" dataDxfId="2"/>
-    <tableColumn id="2" name="Medical Exam Required?" dataDxfId="1"/>
-    <tableColumn id="3" name="SampleRatefor$10000" dataDxfId="0" dataCellStyle="Currency"/>
+    <tableColumn id="1" name="Policy" dataDxfId="13"/>
+    <tableColumn id="2" name="MedicalExamRequired" dataDxfId="12"/>
+    <tableColumn id="3" name="SampleRatefor$10000" dataDxfId="11" dataCellStyle="Currency"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="ProspectsTable" displayName="ProspectsTable" ref="A5:I6" insertRow="1" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A5:I6"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="AgentName" dataDxfId="8"/>
+    <tableColumn id="2" name="ApplicantName" dataDxfId="7"/>
+    <tableColumn id="3" name="Age" dataDxfId="6"/>
+    <tableColumn id="5" name="Gender" dataDxfId="5"/>
+    <tableColumn id="4" name="PolicyName" dataDxfId="4"/>
+    <tableColumn id="6" name="MedicalExamRequired" dataDxfId="3"/>
+    <tableColumn id="7" name="SampleRate" dataDxfId="2"/>
+    <tableColumn id="8" name="InsuranceAmount" dataDxfId="1"/>
+    <tableColumn id="9" name="ApproxMonthlyPayment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -940,7 +1082,7 @@
     <row r="1" spans="1:22" ht="38.25" x14ac:dyDescent="1.1000000000000001">
       <c r="A1" s="5"/>
       <c r="B1" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -989,18 +1131,18 @@
     </row>
     <row r="3" spans="1:22" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A3" s="4"/>
-      <c r="B3" s="12" t="s">
-        <v>34</v>
+      <c r="B3" s="10" t="s">
+        <v>31</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -5539,8 +5681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection sqref="A1:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5553,12 +5695,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.75">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -5578,7 +5720,7 @@
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.65">
       <c r="A3" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -5602,7 +5744,7 @@
     </row>
     <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -5995,12 +6137,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="25.5" x14ac:dyDescent="0.75">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -6058,7 +6200,7 @@
     </row>
     <row r="3" spans="1:28" ht="21" x14ac:dyDescent="0.65">
       <c r="A3" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -6119,7 +6261,7 @@
     </row>
     <row r="5" spans="1:28" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>20</v>
@@ -7894,7 +8036,7 @@
   <dimension ref="A1:D99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:D99"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7906,12 +8048,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.75">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
@@ -7921,7 +8063,7 @@
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.65">
       <c r="A3" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -7938,10 +8080,10 @@
         <v>25</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3"/>
     </row>
@@ -7950,7 +8092,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C6" s="8">
         <v>42.5</v>
@@ -7962,7 +8104,7 @@
         <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C7" s="8">
         <v>35.25</v>
@@ -7974,7 +8116,7 @@
         <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C8" s="8">
         <v>25</v>
@@ -7986,7 +8128,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C9" s="8">
         <v>4.75</v>
@@ -8542,4 +8684,1770 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L198"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="28.46484375" customWidth="1"/>
+    <col min="2" max="2" width="24.73046875" customWidth="1"/>
+    <col min="3" max="4" width="10.9296875" customWidth="1"/>
+    <col min="5" max="5" width="26.59765625" customWidth="1"/>
+    <col min="6" max="6" width="30" customWidth="1"/>
+    <col min="7" max="7" width="12.796875" customWidth="1"/>
+    <col min="8" max="8" width="23.53125" customWidth="1"/>
+    <col min="9" max="9" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="25.5" x14ac:dyDescent="0.75">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.65">
+      <c r="A3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A114" s="4"/>
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A115" s="4"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A116" s="4"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A122" s="4"/>
+      <c r="B122" s="4"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A123" s="4"/>
+      <c r="B123" s="4"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A124" s="4"/>
+      <c r="B124" s="4"/>
+      <c r="C124" s="4"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A125" s="4"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A126" s="4"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A127" s="4"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="4"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="4"/>
+      <c r="F127" s="4"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A128" s="4"/>
+      <c r="B128" s="4"/>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="4"/>
+      <c r="F128" s="4"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A129" s="4"/>
+      <c r="B129" s="4"/>
+      <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="4"/>
+      <c r="F129" s="4"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A130" s="4"/>
+      <c r="B130" s="4"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="4"/>
+      <c r="E130" s="4"/>
+      <c r="F130" s="4"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A131" s="4"/>
+      <c r="B131" s="4"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="4"/>
+      <c r="F131" s="4"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A132" s="4"/>
+      <c r="B132" s="4"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="4"/>
+      <c r="F132" s="4"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A133" s="4"/>
+      <c r="B133" s="4"/>
+      <c r="C133" s="4"/>
+      <c r="D133" s="4"/>
+      <c r="E133" s="4"/>
+      <c r="F133" s="4"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A134" s="4"/>
+      <c r="B134" s="4"/>
+      <c r="C134" s="4"/>
+      <c r="D134" s="4"/>
+      <c r="E134" s="4"/>
+      <c r="F134" s="4"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A135" s="4"/>
+      <c r="B135" s="4"/>
+      <c r="C135" s="4"/>
+      <c r="D135" s="4"/>
+      <c r="E135" s="4"/>
+      <c r="F135" s="4"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A136" s="4"/>
+      <c r="B136" s="4"/>
+      <c r="C136" s="4"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="4"/>
+      <c r="F136" s="4"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A137" s="4"/>
+      <c r="B137" s="4"/>
+      <c r="C137" s="4"/>
+      <c r="D137" s="4"/>
+      <c r="E137" s="4"/>
+      <c r="F137" s="4"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A138" s="4"/>
+      <c r="B138" s="4"/>
+      <c r="C138" s="4"/>
+      <c r="D138" s="4"/>
+      <c r="E138" s="4"/>
+      <c r="F138" s="4"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A139" s="4"/>
+      <c r="B139" s="4"/>
+      <c r="C139" s="4"/>
+      <c r="D139" s="4"/>
+      <c r="E139" s="4"/>
+      <c r="F139" s="4"/>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A140" s="4"/>
+      <c r="B140" s="4"/>
+      <c r="C140" s="4"/>
+      <c r="D140" s="4"/>
+      <c r="E140" s="4"/>
+      <c r="F140" s="4"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A141" s="4"/>
+      <c r="B141" s="4"/>
+      <c r="C141" s="4"/>
+      <c r="D141" s="4"/>
+      <c r="E141" s="4"/>
+      <c r="F141" s="4"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A142" s="4"/>
+      <c r="B142" s="4"/>
+      <c r="C142" s="4"/>
+      <c r="D142" s="4"/>
+      <c r="E142" s="4"/>
+      <c r="F142" s="4"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A143" s="4"/>
+      <c r="B143" s="4"/>
+      <c r="C143" s="4"/>
+      <c r="D143" s="4"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="4"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A144" s="4"/>
+      <c r="B144" s="4"/>
+      <c r="C144" s="4"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A145" s="4"/>
+      <c r="B145" s="4"/>
+      <c r="C145" s="4"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A146" s="4"/>
+      <c r="B146" s="4"/>
+      <c r="C146" s="4"/>
+      <c r="D146" s="4"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4"/>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A147" s="4"/>
+      <c r="B147" s="4"/>
+      <c r="C147" s="4"/>
+      <c r="D147" s="4"/>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A148" s="4"/>
+      <c r="B148" s="4"/>
+      <c r="C148" s="4"/>
+      <c r="D148" s="4"/>
+      <c r="E148" s="4"/>
+      <c r="F148" s="4"/>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A149" s="4"/>
+      <c r="B149" s="4"/>
+      <c r="C149" s="4"/>
+      <c r="D149" s="4"/>
+      <c r="E149" s="4"/>
+      <c r="F149" s="4"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A150" s="4"/>
+      <c r="B150" s="4"/>
+      <c r="C150" s="4"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A151" s="4"/>
+      <c r="B151" s="4"/>
+      <c r="C151" s="4"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="4"/>
+      <c r="F151" s="4"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A152" s="4"/>
+      <c r="B152" s="4"/>
+      <c r="C152" s="4"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A153" s="4"/>
+      <c r="B153" s="4"/>
+      <c r="C153" s="4"/>
+      <c r="D153" s="4"/>
+      <c r="E153" s="4"/>
+      <c r="F153" s="4"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A154" s="4"/>
+      <c r="B154" s="4"/>
+      <c r="C154" s="4"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="4"/>
+      <c r="F154" s="4"/>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A155" s="4"/>
+      <c r="B155" s="4"/>
+      <c r="C155" s="4"/>
+      <c r="D155" s="4"/>
+      <c r="E155" s="4"/>
+      <c r="F155" s="4"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A156" s="4"/>
+      <c r="B156" s="4"/>
+      <c r="C156" s="4"/>
+      <c r="D156" s="4"/>
+      <c r="E156" s="4"/>
+      <c r="F156" s="4"/>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A157" s="4"/>
+      <c r="B157" s="4"/>
+      <c r="C157" s="4"/>
+      <c r="D157" s="4"/>
+      <c r="E157" s="4"/>
+      <c r="F157" s="4"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A158" s="4"/>
+      <c r="B158" s="4"/>
+      <c r="C158" s="4"/>
+      <c r="D158" s="4"/>
+      <c r="E158" s="4"/>
+      <c r="F158" s="4"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A159" s="4"/>
+      <c r="B159" s="4"/>
+      <c r="C159" s="4"/>
+      <c r="D159" s="4"/>
+      <c r="E159" s="4"/>
+      <c r="F159" s="4"/>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A160" s="4"/>
+      <c r="B160" s="4"/>
+      <c r="C160" s="4"/>
+      <c r="D160" s="4"/>
+      <c r="E160" s="4"/>
+      <c r="F160" s="4"/>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A161" s="4"/>
+      <c r="B161" s="4"/>
+      <c r="C161" s="4"/>
+      <c r="D161" s="4"/>
+      <c r="E161" s="4"/>
+      <c r="F161" s="4"/>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A162" s="4"/>
+      <c r="B162" s="4"/>
+      <c r="C162" s="4"/>
+      <c r="D162" s="4"/>
+      <c r="E162" s="4"/>
+      <c r="F162" s="4"/>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A163" s="4"/>
+      <c r="B163" s="4"/>
+      <c r="C163" s="4"/>
+      <c r="D163" s="4"/>
+      <c r="E163" s="4"/>
+      <c r="F163" s="4"/>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A164" s="4"/>
+      <c r="B164" s="4"/>
+      <c r="C164" s="4"/>
+      <c r="D164" s="4"/>
+      <c r="E164" s="4"/>
+      <c r="F164" s="4"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A165" s="4"/>
+      <c r="B165" s="4"/>
+      <c r="C165" s="4"/>
+      <c r="D165" s="4"/>
+      <c r="E165" s="4"/>
+      <c r="F165" s="4"/>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A166" s="4"/>
+      <c r="B166" s="4"/>
+      <c r="C166" s="4"/>
+      <c r="D166" s="4"/>
+      <c r="E166" s="4"/>
+      <c r="F166" s="4"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A167" s="4"/>
+      <c r="B167" s="4"/>
+      <c r="C167" s="4"/>
+      <c r="D167" s="4"/>
+      <c r="E167" s="4"/>
+      <c r="F167" s="4"/>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A168" s="4"/>
+      <c r="B168" s="4"/>
+      <c r="C168" s="4"/>
+      <c r="D168" s="4"/>
+      <c r="E168" s="4"/>
+      <c r="F168" s="4"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A169" s="4"/>
+      <c r="B169" s="4"/>
+      <c r="C169" s="4"/>
+      <c r="D169" s="4"/>
+      <c r="E169" s="4"/>
+      <c r="F169" s="4"/>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A170" s="4"/>
+      <c r="B170" s="4"/>
+      <c r="C170" s="4"/>
+      <c r="D170" s="4"/>
+      <c r="E170" s="4"/>
+      <c r="F170" s="4"/>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A171" s="4"/>
+      <c r="B171" s="4"/>
+      <c r="C171" s="4"/>
+      <c r="D171" s="4"/>
+      <c r="E171" s="4"/>
+      <c r="F171" s="4"/>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A172" s="4"/>
+      <c r="B172" s="4"/>
+      <c r="C172" s="4"/>
+      <c r="D172" s="4"/>
+      <c r="E172" s="4"/>
+      <c r="F172" s="4"/>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A173" s="4"/>
+      <c r="B173" s="4"/>
+      <c r="C173" s="4"/>
+      <c r="D173" s="4"/>
+      <c r="E173" s="4"/>
+      <c r="F173" s="4"/>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A174" s="4"/>
+      <c r="B174" s="4"/>
+      <c r="C174" s="4"/>
+      <c r="D174" s="4"/>
+      <c r="E174" s="4"/>
+      <c r="F174" s="4"/>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A175" s="4"/>
+      <c r="B175" s="4"/>
+      <c r="C175" s="4"/>
+      <c r="D175" s="4"/>
+      <c r="E175" s="4"/>
+      <c r="F175" s="4"/>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A176" s="4"/>
+      <c r="B176" s="4"/>
+      <c r="C176" s="4"/>
+      <c r="D176" s="4"/>
+      <c r="E176" s="4"/>
+      <c r="F176" s="4"/>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A177" s="4"/>
+      <c r="B177" s="4"/>
+      <c r="C177" s="4"/>
+      <c r="D177" s="4"/>
+      <c r="E177" s="4"/>
+      <c r="F177" s="4"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A178" s="4"/>
+      <c r="B178" s="4"/>
+      <c r="C178" s="4"/>
+      <c r="D178" s="4"/>
+      <c r="E178" s="4"/>
+      <c r="F178" s="4"/>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A179" s="4"/>
+      <c r="B179" s="4"/>
+      <c r="C179" s="4"/>
+      <c r="D179" s="4"/>
+      <c r="E179" s="4"/>
+      <c r="F179" s="4"/>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A180" s="4"/>
+      <c r="B180" s="4"/>
+      <c r="C180" s="4"/>
+      <c r="D180" s="4"/>
+      <c r="E180" s="4"/>
+      <c r="F180" s="4"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A181" s="4"/>
+      <c r="B181" s="4"/>
+      <c r="C181" s="4"/>
+      <c r="D181" s="4"/>
+      <c r="E181" s="4"/>
+      <c r="F181" s="4"/>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A182" s="4"/>
+      <c r="B182" s="4"/>
+      <c r="C182" s="4"/>
+      <c r="D182" s="4"/>
+      <c r="E182" s="4"/>
+      <c r="F182" s="4"/>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A183" s="4"/>
+      <c r="B183" s="4"/>
+      <c r="C183" s="4"/>
+      <c r="D183" s="4"/>
+      <c r="E183" s="4"/>
+      <c r="F183" s="4"/>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A184" s="4"/>
+      <c r="B184" s="4"/>
+      <c r="C184" s="4"/>
+      <c r="D184" s="4"/>
+      <c r="E184" s="4"/>
+      <c r="F184" s="4"/>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A185" s="4"/>
+      <c r="B185" s="4"/>
+      <c r="C185" s="4"/>
+      <c r="D185" s="4"/>
+      <c r="E185" s="4"/>
+      <c r="F185" s="4"/>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A186" s="4"/>
+      <c r="B186" s="4"/>
+      <c r="C186" s="4"/>
+      <c r="D186" s="4"/>
+      <c r="E186" s="4"/>
+      <c r="F186" s="4"/>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A187" s="4"/>
+      <c r="B187" s="4"/>
+      <c r="C187" s="4"/>
+      <c r="D187" s="4"/>
+      <c r="E187" s="4"/>
+      <c r="F187" s="4"/>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A188" s="4"/>
+      <c r="B188" s="4"/>
+      <c r="C188" s="4"/>
+      <c r="D188" s="4"/>
+      <c r="E188" s="4"/>
+      <c r="F188" s="4"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A189" s="4"/>
+      <c r="B189" s="4"/>
+      <c r="C189" s="4"/>
+      <c r="D189" s="4"/>
+      <c r="E189" s="4"/>
+      <c r="F189" s="4"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A190" s="4"/>
+      <c r="B190" s="4"/>
+      <c r="C190" s="4"/>
+      <c r="D190" s="4"/>
+      <c r="E190" s="4"/>
+      <c r="F190" s="4"/>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A191" s="4"/>
+      <c r="B191" s="4"/>
+      <c r="C191" s="4"/>
+      <c r="D191" s="4"/>
+      <c r="E191" s="4"/>
+      <c r="F191" s="4"/>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A192" s="4"/>
+      <c r="B192" s="4"/>
+      <c r="C192" s="4"/>
+      <c r="D192" s="4"/>
+      <c r="E192" s="4"/>
+      <c r="F192" s="4"/>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A193" s="4"/>
+      <c r="B193" s="4"/>
+      <c r="C193" s="4"/>
+      <c r="D193" s="4"/>
+      <c r="E193" s="4"/>
+      <c r="F193" s="4"/>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A194" s="4"/>
+      <c r="B194" s="4"/>
+      <c r="C194" s="4"/>
+      <c r="D194" s="4"/>
+      <c r="E194" s="4"/>
+      <c r="F194" s="4"/>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A195" s="4"/>
+      <c r="B195" s="4"/>
+      <c r="C195" s="4"/>
+      <c r="D195" s="4"/>
+      <c r="E195" s="4"/>
+      <c r="F195" s="4"/>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A196" s="4"/>
+      <c r="B196" s="4"/>
+      <c r="C196" s="4"/>
+      <c r="D196" s="4"/>
+      <c r="E196" s="4"/>
+      <c r="F196" s="4"/>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A197" s="4"/>
+      <c r="B197" s="4"/>
+      <c r="C197" s="4"/>
+      <c r="D197" s="4"/>
+      <c r="E197" s="4"/>
+      <c r="F197" s="4"/>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A198" s="4"/>
+      <c r="B198" s="4"/>
+      <c r="C198" s="4"/>
+      <c r="D198" s="4"/>
+      <c r="E198" s="4"/>
+      <c r="F198" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating it to the latest
</commit_message>
<xml_diff>
--- a/HumongousInsuranceAgentsAddin/HumongousInsuranceAgentsAddin/HumongousInsuranceExcelSpreadsheet.xlsx
+++ b/HumongousInsuranceAgentsAddin/HumongousInsuranceAgentsAddin/HumongousInsuranceExcelSpreadsheet.xlsx
@@ -296,8 +296,8 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="7" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
@@ -1071,41 +1071,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V191"/>
+  <dimension ref="A1:X191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="38.25" x14ac:dyDescent="1.1000000000000001">
+    <row r="1" spans="1:24" ht="38.25" x14ac:dyDescent="1.1000000000000001">
       <c r="A1" s="5"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1129,20 +1131,20 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:22" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:24" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A3" s="4"/>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -1155,7 +1157,7 @@
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1179,7 +1181,7 @@
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1203,7 +1205,7 @@
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1227,7 +1229,7 @@
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1251,7 +1253,7 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1275,7 +1277,7 @@
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1299,7 +1301,7 @@
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1323,7 +1325,7 @@
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1347,7 +1349,7 @@
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1371,7 +1373,7 @@
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1395,7 +1397,7 @@
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1419,7 +1421,7 @@
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1443,7 +1445,7 @@
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -5669,8 +5671,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:K1"/>
     <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B1:X1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5681,8 +5683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection sqref="A1:D36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>